<commit_message>
Ajustes no dicionário de dados
</commit_message>
<xml_diff>
--- a/Dicionário de dados/dicionario_tabela_op.xlsx
+++ b/Dicionário de dados/dicionario_tabela_op.xlsx
@@ -1,25 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\supor\OneDrive\Área de Trabalho\TrabalhoBD\Dicionário de dados\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF3FE41-B25A-4828-9969-D59A07EC449A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{352D6D85-AE48-4FB0-AD2D-6C5E4B5751E1}"/>
+    <workbookView windowWidth="23040" windowHeight="8555"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -41,9 +32,15 @@
     <t>Tabela</t>
   </si>
   <si>
+    <t>OP</t>
+  </si>
+  <si>
     <t>Descrição</t>
   </si>
   <si>
+    <t>Tabela responsável por armazenar dados completos das operações de produção</t>
+  </si>
+  <si>
     <t>Atributos</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
     <t>FK</t>
   </si>
   <si>
+    <t>id_op</t>
+  </si>
+  <si>
     <t>SERIAL</t>
   </si>
   <si>
@@ -77,73 +77,64 @@
     <t>X</t>
   </si>
   <si>
+    <t xml:space="preserve"> Codigo identificador da ordem de produção</t>
+  </si>
+  <si>
+    <t>data_inicio</t>
+  </si>
+  <si>
+    <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>1 - sem limite</t>
+  </si>
+  <si>
+    <t>Data inicial da ordem de produção</t>
+  </si>
+  <si>
+    <t>data_conclusao</t>
+  </si>
+  <si>
+    <t>Data final da ordem de produção</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 - 50 </t>
+  </si>
+  <si>
+    <t>Status em que a ordem de produção  se encontra</t>
+  </si>
+  <si>
+    <t>quantidade_a_produzir</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>Quantidade de determinado produto sera produzido</t>
+  </si>
+  <si>
     <t>id_produto</t>
   </si>
   <si>
-    <t>INT</t>
-  </si>
-  <si>
-    <t>1 - sem limite</t>
-  </si>
-  <si>
-    <t>OP</t>
-  </si>
-  <si>
-    <t>id_op</t>
-  </si>
-  <si>
-    <t>data_inicio</t>
-  </si>
-  <si>
-    <t>TIMESTAMP</t>
-  </si>
-  <si>
-    <t>data_conclusao</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>VARCHAR(50)</t>
-  </si>
-  <si>
-    <t>quantidade_a_produzir</t>
-  </si>
-  <si>
-    <t>Quantidade de determinado produto sera produzido</t>
-  </si>
-  <si>
     <t>ID do produto que sera produzido</t>
   </si>
   <si>
     <t>data_de_criacao</t>
   </si>
   <si>
+    <t>Data em que a ordem de produção foi criada</t>
+  </si>
+  <si>
     <t>data_de_atualizacao</t>
   </si>
   <si>
-    <t>Tabela responsável por armazenar dados completos das operações de produção</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Codigo identificador da ordem de produção</t>
-  </si>
-  <si>
-    <t>Data inicial da ordem de produção</t>
-  </si>
-  <si>
-    <t>Data final da ordem de produção</t>
-  </si>
-  <si>
-    <t>Status em que a ordem de produção  se encontra</t>
-  </si>
-  <si>
     <t>Data em que foi realizada alguma alteração/atualização referente a ordem de produção</t>
-  </si>
-  <si>
-    <t>Data em que a ordem de produção foi criada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 - 50 </t>
   </si>
   <si>
     <t>valor_final</t>
@@ -161,13 +152,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -175,14 +172,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFA6A6A6"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -190,11 +187,162 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,8 +355,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -218,50 +552,292 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -269,37 +845,78 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
+    <cellStyle name="Porcentagem" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moeda [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Hyperlink seguido" xfId="7" builtinId="9"/>
+    <cellStyle name="Observação" xfId="8" builtinId="10"/>
+    <cellStyle name="Texto de Aviso" xfId="9" builtinId="11"/>
+    <cellStyle name="Título" xfId="10" builtinId="15"/>
+    <cellStyle name="Texto Explicativo" xfId="11" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
+    <cellStyle name="Saída" xfId="17" builtinId="21"/>
+    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
+    <cellStyle name="Célula de Verificação" xfId="19" builtinId="23"/>
+    <cellStyle name="Célula Vinculada" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Bom" xfId="22" builtinId="26"/>
+    <cellStyle name="Ruim" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
+    <cellStyle name="Ênfase 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Ênfase 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Ênfase 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Ênfase 1" xfId="28" builtinId="32"/>
+    <cellStyle name="Ênfase 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Ênfase 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Ênfase 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Ênfase 2" xfId="32" builtinId="36"/>
+    <cellStyle name="Ênfase 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Ênfase 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Ênfase 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Ênfase 3" xfId="36" builtinId="40"/>
+    <cellStyle name="Ênfase 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Ênfase 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Ênfase 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Ênfase 4" xfId="40" builtinId="44"/>
+    <cellStyle name="Ênfase 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Ênfase 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Ênfase 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Ênfase 5" xfId="44" builtinId="48"/>
+    <cellStyle name="Ênfase 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Ênfase 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Ênfase 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -348,7 +965,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -381,26 +998,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -433,23 +1033,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -611,267 +1194,262 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44FB5DF-5950-44ED-A8D0-ADFDA4A2D838}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="64.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="16.8518518518519" customWidth="1"/>
+    <col min="3" max="3" width="14.8518518518519" customWidth="1"/>
+    <col min="4" max="4" width="14.5740740740741" customWidth="1"/>
+    <col min="5" max="5" width="15.287037037037" customWidth="1"/>
+    <col min="8" max="8" width="64.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" ht="28.8" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="9"/>
+    <row r="5" ht="28.8" spans="1:11">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" ht="28.8" spans="1:8">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="5"/>
+    <row r="7" ht="28.8" spans="1:8">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5"/>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>35</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="5"/>
+    <row r="9" ht="28.8" spans="1:8">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="5"/>
+    <row r="10" ht="28.8" spans="1:8">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="5"/>
+    <row r="11" ht="28.8" spans="1:8">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" ht="28.8" spans="1:8">
+      <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>37</v>
       </c>
@@ -879,7 +1457,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -887,13 +1465,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="3"/>
+    <row r="24" spans="8:8">
+      <c r="H24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
@@ -905,7 +1481,10 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>